<commit_message>
Task 1 - some minor print mods
</commit_message>
<xml_diff>
--- a/task1.xlsx
+++ b/task1.xlsx
@@ -765,7 +765,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="100" workbookViewId="0">
       <selection activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -836,7 +836,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
@@ -880,7 +880,7 @@
       </c>
       <c r="H16" s="11">
         <f>_xlfn.BINOM.DIST(k,n,p,0)</f>
-        <v>0.23213428125000013</v>
+        <v>0.04062349921875006</v>
       </c>
     </row>
     <row r="17">
@@ -904,7 +904,7 @@
       </c>
       <c r="H18" s="11">
         <f>_xlfn.BINOM.DIST(k_2,n,p,1)-_xlfn.BINOM.DIST(k_1,n,p,1)+_xlfn.BINOM.DIST(k_1,n,p,0)</f>
-        <v>0.26267826562500018</v>
+        <v>0.044186964062500063</v>
       </c>
     </row>
     <row r="19">
@@ -925,7 +925,7 @@
       </c>
       <c r="H20" s="11">
         <f>_xlfn.BINOM.DIST(k_3,n,p,1)</f>
-        <v>8.6406250000000315e-05</v>
+        <v>6.0273437500000275e-06</v>
       </c>
     </row>
     <row r="21">
@@ -946,7 +946,7 @@
       </c>
       <c r="H22" s="11">
         <f>1-_xlfn.BINOM.DIST(k_4,n,p,1)+_xlfn.BINOM.DIST(k_4,n,p,0)</f>
-        <v>0.96722617187499993</v>
+        <v>0.99624295703124999</v>
       </c>
     </row>
     <row r="24">
@@ -955,7 +955,7 @@
       </c>
       <c r="H24" s="11">
         <f>1-_xlfn.BINOM.DIST(0,n,p,0)</f>
-        <v>0.99999998437500004</v>
+        <v>0.99999999921875005</v>
       </c>
     </row>
     <row r="26">
@@ -964,21 +964,21 @@
       </c>
       <c r="D26">
         <f>n*p-q</f>
-        <v>5.6499999999999995</v>
+        <v>6.5999999999999996</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F26">
         <f>n*p+p</f>
-        <v>6.6499999999999995</v>
+        <v>7.5999999999999996</v>
       </c>
       <c r="G26" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="12">
         <f>ROUNDUP(D26,0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
@@ -987,7 +987,7 @@
       </c>
       <c r="H27" s="11">
         <f>_xlfn.BINOM.DIST(H26,n,p,0)</f>
-        <v>0.7350918906249998</v>
+        <v>0.69833729609374973</v>
       </c>
     </row>
   </sheetData>

</xml_diff>